<commit_message>
Compatible with RevB software under RevC hardware
</commit_message>
<xml_diff>
--- a/Hardware Docs/RevC SCH and Gerber/SDP-B GPIO REVC.xlsx
+++ b/Hardware Docs/RevC SCH and Gerber/SDP-B GPIO REVC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Signal Define" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="136">
   <si>
     <t>GPIO2</t>
   </si>
@@ -114,15 +114,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>-15V</t>
-  </si>
-  <si>
-    <t>+15V</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -147,12 +138,6 @@
     <t>Set 5</t>
   </si>
   <si>
-    <t>Set 6</t>
-  </si>
-  <si>
-    <t>Set 7</t>
-  </si>
-  <si>
     <t>Set 8</t>
   </si>
   <si>
@@ -165,24 +150,12 @@
     <t>AIN -----VREF</t>
   </si>
   <si>
-    <t>CONFIG----VCS</t>
-  </si>
-  <si>
-    <t>CONFIG----VREF</t>
-  </si>
-  <si>
     <t>AIN-----VOUT</t>
   </si>
   <si>
-    <t>AIN-----510OUT</t>
-  </si>
-  <si>
     <t>CONFIG----VOUT</t>
   </si>
   <si>
-    <t>CONFIG----510OUT</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -192,18 +165,12 @@
     <t>VREF Measure</t>
   </si>
   <si>
-    <t>510OUT Measure</t>
-  </si>
-  <si>
     <t>VOUT Measure</t>
   </si>
   <si>
     <t>Digital Control</t>
   </si>
   <si>
-    <t>+/-15V Digital Control</t>
-  </si>
-  <si>
     <t>CON</t>
   </si>
   <si>
@@ -231,9 +198,6 @@
     <t>5V</t>
   </si>
   <si>
-    <t>6V</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -243,12 +207,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>AIN-----MOUT</t>
-  </si>
-  <si>
-    <t>MOUT Measure</t>
-  </si>
-  <si>
     <t>Set 9</t>
   </si>
   <si>
@@ -361,6 +319,111 @@
   </si>
   <si>
     <t>GPIO09</t>
+  </si>
+  <si>
+    <t>Vout/Vref with/without Cap</t>
+  </si>
+  <si>
+    <t>CONFIG with buffer/bypass</t>
+  </si>
+  <si>
+    <t>with buffer</t>
+  </si>
+  <si>
+    <t>bypass</t>
+  </si>
+  <si>
+    <t>without</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>VOUT to CONFIG/AVOUT</t>
+  </si>
+  <si>
+    <t>to CONFIG</t>
+  </si>
+  <si>
+    <t>to AVOUT</t>
+  </si>
+  <si>
+    <t>to AVOUT/MLVOUT</t>
+  </si>
+  <si>
+    <t>to VCS/VREF</t>
+  </si>
+  <si>
+    <t>AVOUT/MLVOUT or VCS/VREF</t>
+  </si>
+  <si>
+    <t>ADC to AVOUT/VCS or MLVOUT/VREF</t>
+  </si>
+  <si>
+    <t>to AVOUT/VCS</t>
+  </si>
+  <si>
+    <t>to MLVOUT/VREF</t>
+  </si>
+  <si>
+    <t>+/-15V ON/OFF</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>VDD from 6VFUSE/others</t>
+  </si>
+  <si>
+    <t>6VFUSE</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>others power is GND/5V4V5</t>
+  </si>
+  <si>
+    <t>5V4V5</t>
+  </si>
+  <si>
+    <t>5V4V5 is 5V/4V5</t>
+  </si>
+  <si>
+    <t>4V5</t>
+  </si>
+  <si>
+    <t>GPIO6</t>
+  </si>
+  <si>
+    <t>+/-15V</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
+  </si>
+  <si>
+    <t>VOUT and VREF with Cap</t>
+  </si>
+  <si>
+    <t>VOUT and VREF without Cap</t>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>digital control</t>
+  </si>
+  <si>
+    <t>analog output</t>
+  </si>
+  <si>
+    <t>AIN-----MLVOUT</t>
+  </si>
+  <si>
+    <t>MLVOUT/MOUT Measure</t>
   </si>
 </sst>
 </file>
@@ -384,7 +447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,12 +456,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -415,11 +484,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,7 +511,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,8 +518,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,8 +623,8 @@
     <tableColumn id="1" name="IO Name"/>
     <tableColumn id="2" name="GPIO2"/>
     <tableColumn id="3" name="GPIO3"/>
-    <tableColumn id="4" name="GPIO11"/>
-    <tableColumn id="8" name="GPIO4"/>
+    <tableColumn id="4" name="GPIO4"/>
+    <tableColumn id="8" name="GPIO5"/>
     <tableColumn id="5" name="Signal Path "/>
     <tableColumn id="6" name="Mode"/>
     <tableColumn id="7" name="Note"/>
@@ -546,16 +634,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="表8" displayName="表8" ref="A2:G9" totalsRowShown="0">
-  <autoFilter ref="A2:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="表8" displayName="表8" ref="A2:G8" totalsRowShown="0">
+  <autoFilter ref="A2:G8"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Power"/>
     <tableColumn id="2" name="Voltage"/>
     <tableColumn id="3" name="Status"/>
-    <tableColumn id="4" name="GPIO7"/>
-    <tableColumn id="5" name="GPIO8"/>
-    <tableColumn id="6" name="GPIO9"/>
-    <tableColumn id="7" name="GPIO10"/>
+    <tableColumn id="4" name="GPIO6"/>
+    <tableColumn id="5" name="GPIO7"/>
+    <tableColumn id="6" name="GPIO8"/>
+    <tableColumn id="7" name="GPIO9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -850,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +948,7 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -869,7 +957,7 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -892,7 +980,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -901,15 +989,21 @@
         <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -918,15 +1012,21 @@
         <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -935,15 +1035,21 @@
         <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -952,15 +1058,21 @@
         <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -969,83 +1081,113 @@
         <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="11">
         <v>47</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="D8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="11">
         <v>74</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="D9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="11">
         <v>43</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="D10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="11">
         <v>44</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="D11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
@@ -1056,16 +1198,16 @@
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3">
         <v>37</v>
@@ -1073,16 +1215,16 @@
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3">
         <v>38</v>
@@ -1090,13 +1232,13 @@
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
@@ -1107,11 +1249,11 @@
       <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
@@ -1122,11 +1264,11 @@
       <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>16</v>
@@ -1137,228 +1279,228 @@
       <c r="D17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3">
         <v>85</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3">
         <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3">
         <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>68</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3">
         <v>88</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3">
         <v>92</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3">
         <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3">
         <v>32</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C25" s="3">
         <v>87</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C26" s="3">
         <v>35</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C27" s="3">
         <v>89</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="E27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C28" s="3">
         <v>90</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3">
         <v>91</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3">
         <v>41</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
@@ -1376,7 +1518,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E3:E7"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,8 +1528,8 @@
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1402,243 +1544,197 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>50</v>
+        <v>131</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="5"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
+      <c r="G7" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>61</v>
+        <v>130</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G9"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,174 +1750,151 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v4.2 fix GPIOs, GPIO20 is useless
</commit_message>
<xml_diff>
--- a/Hardware Docs/RevC SCH and Gerber/SDP-B GPIO REVC.xlsx
+++ b/Hardware Docs/RevC SCH and Gerber/SDP-B GPIO REVC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Signal Define" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="142">
   <si>
     <t>GPIO2</t>
   </si>
@@ -424,6 +424,24 @@
   </si>
   <si>
     <t>MLVOUT/MOUT Measure</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>EPIO5</t>
+  </si>
+  <si>
+    <t>EPIO4</t>
+  </si>
+  <si>
+    <t>EPIO3</t>
+  </si>
+  <si>
+    <t>EPIO1</t>
+  </si>
+  <si>
+    <t>EPIO2</t>
   </si>
 </sst>
 </file>
@@ -938,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1331,9 @@
       <c r="D19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
@@ -1330,7 +1350,9 @@
       <c r="D20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
@@ -1347,7 +1369,9 @@
       <c r="D21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
@@ -1364,7 +1388,9 @@
       <c r="D22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
@@ -1381,7 +1407,9 @@
       <c r="D23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
@@ -1398,7 +1426,9 @@
       <c r="D24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
@@ -1733,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>